<commit_message>
Testiranje izjava i pokrivenosti
</commit_message>
<xml_diff>
--- a/Testiranje izjava i pokrivenost.xlsx
+++ b/Testiranje izjava i pokrivenost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenoa\Desktop\Github\Formalne-Metode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E26F57-2DF6-442E-81B9-02AB06D5D3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4994F6C6-9903-47C7-9B06-0DCFCBAFD0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Test slučaj</t>
   </si>
@@ -49,21 +49,6 @@
   </si>
   <si>
     <t>poziv funkcije PrikaziSveDokumente()</t>
-  </si>
-  <si>
-    <t>poziv funkcije FiltrirajDokumente("FM", "", "")</t>
-  </si>
-  <si>
-    <t>"Vježbe"</t>
-  </si>
-  <si>
-    <t>poziv funkcije FiltrirajDokumente("", "Vježbe", "")</t>
-  </si>
-  <si>
-    <t>"2022/2023"</t>
-  </si>
-  <si>
-    <t>poziv funkcije FiltrirajDokumente("", "", "2022/2023")</t>
   </si>
   <si>
     <t>"2021/2022"</t>
@@ -220,6 +205,85 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>605118</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1770530</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59EE8D77-2D34-5E1D-5F49-B147426F3B42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12102353" y="1748118"/>
+          <a:ext cx="4784912" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Da bi se pokrile sve linije koda potrebno je izvr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="bs-Latn-BA" sz="1100"/>
+            <a:t>šiti</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="bs-Latn-BA" sz="1100" baseline="0"/>
+            <a:t> test slučajeve iz tabele.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -486,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="T4:X19"/>
+  <dimension ref="T4:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -543,13 +607,13 @@
         <v>5</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="20:24">
@@ -559,93 +623,21 @@
       <c r="U7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="6" t="s">
-        <v>9</v>
+      <c r="V7" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="20:24">
-      <c r="T8" s="4">
-        <v>4</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="W8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="T8" s="3"/>
     </row>
     <row r="9" spans="20:24">
-      <c r="T9" s="4">
-        <v>5</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="V9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="W9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="20:24">
-      <c r="T10" s="4">
-        <v>6</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="V10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="W10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="X10" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="20:24">
-      <c r="T11" s="3"/>
-    </row>
-    <row r="12" spans="20:24">
-      <c r="T12" s="3"/>
-    </row>
-    <row r="13" spans="20:24">
-      <c r="T13" s="3"/>
-    </row>
-    <row r="14" spans="20:24">
-      <c r="T14" s="3"/>
-    </row>
-    <row r="15" spans="20:24">
-      <c r="T15" s="3"/>
-    </row>
-    <row r="16" spans="20:24">
-      <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="20:20">
-      <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="20:20">
-      <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="20:20">
-      <c r="T19" s="3"/>
+      <c r="T9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>